<commit_message>
Updated burn report to reflect time worked on initial web dev for rover submodule web interface
</commit_message>
<xml_diff>
--- a/team_folder/newFolder/Project Management/Logging/Burn Report.xlsx
+++ b/team_folder/newFolder/Project Management/Logging/Burn Report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
   <si>
     <t xml:space="preserve">Per Person</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t xml:space="preserve">Wrote functional test including sensor, imu and motor components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Begun initial work on web interface of rover with straight, left, right, backward, and 360 buttons</t>
   </si>
   <si>
     <t xml:space="preserve">Total CDR Costs</t>
@@ -794,7 +797,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B41" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
-      <selection pane="topRight" activeCell="I59" activeCellId="0" sqref="I59"/>
+      <selection pane="topRight" activeCell="I60" activeCellId="0" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
@@ -1125,7 +1128,7 @@
       </c>
       <c r="AI4" s="19" t="n">
         <f aca="false">R83-AI3</f>
-        <v>950</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1408,7 +1411,7 @@
       </c>
       <c r="AI7" s="29" t="n">
         <f aca="false">Z83-AI6</f>
-        <v>9.5</v>
+        <v>10.25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1587,7 +1590,7 @@
       </c>
       <c r="AI9" s="19" t="n">
         <f aca="false">SUM(AI3+AI4)</f>
-        <v>1800</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,7 +1692,7 @@
       </c>
       <c r="AI10" s="29" t="n">
         <f aca="false">SUM(AI6+AI7)</f>
-        <v>18</v>
+        <v>18.75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5306,19 +5309,27 @@
       </c>
       <c r="AA58" s="3"/>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="25"/>
-      <c r="B59" s="28"/>
-      <c r="C59" s="23"/>
+    <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="25" t="n">
+        <v>43207</v>
+      </c>
+      <c r="B59" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" s="23" t="n">
+        <v>0.75</v>
+      </c>
       <c r="D59" s="33"/>
       <c r="E59" s="33"/>
       <c r="F59" s="33"/>
       <c r="G59" s="33"/>
       <c r="H59" s="33"/>
-      <c r="I59" s="33"/>
+      <c r="I59" s="33" t="n">
+        <v>1</v>
+      </c>
       <c r="J59" s="18" t="n">
         <f aca="false">SUM(D59:I59)*100*C59</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="L59" s="3"/>
       <c r="M59" s="3" t="n">
@@ -5343,7 +5354,7 @@
       </c>
       <c r="R59" s="3" t="n">
         <f aca="false">IF(I59=1,100*$C59,0)</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="S59" s="3"/>
       <c r="T59" s="3"/>
@@ -5369,7 +5380,7 @@
       </c>
       <c r="Z59" s="24" t="n">
         <f aca="false">IF(I59=1,$C59,0)</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AA59" s="3"/>
     </row>
@@ -6552,7 +6563,7 @@
         <v>0</v>
       </c>
       <c r="S77" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="T77" s="3"/>
       <c r="U77" s="24" t="n">
@@ -6580,7 +6591,7 @@
         <v>0</v>
       </c>
       <c r="AA77" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6624,7 +6635,7 @@
       </c>
       <c r="S78" s="4" t="n">
         <f aca="false">S83-S43</f>
-        <v>1750</v>
+        <v>1825</v>
       </c>
       <c r="T78" s="3"/>
       <c r="U78" s="24" t="n">
@@ -6653,7 +6664,7 @@
       </c>
       <c r="AA78" s="3" t="n">
         <f aca="false">AA83-AA43</f>
-        <v>17.5</v>
+        <v>18.25</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6927,11 +6938,11 @@
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="35"/>
       <c r="B83" s="36" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C83" s="37" t="n">
         <f aca="false">SUM(C3:C82)</f>
-        <v>63.25</v>
+        <v>64</v>
       </c>
       <c r="D83" s="38" t="n">
         <f aca="false">U$83</f>
@@ -6955,14 +6966,14 @@
       </c>
       <c r="I83" s="38" t="n">
         <f aca="false">Z$83</f>
-        <v>18</v>
+        <v>18.75</v>
       </c>
       <c r="J83" s="39" t="n">
         <f aca="false">SUM(J3:J82)</f>
-        <v>6975</v>
+        <v>7050</v>
       </c>
       <c r="L83" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M83" s="4" t="n">
         <f aca="false">SUM(M3:M82)</f>
@@ -6986,11 +6997,11 @@
       </c>
       <c r="R83" s="4" t="n">
         <f aca="false">SUM(R3:R82)</f>
-        <v>1800</v>
+        <v>1875</v>
       </c>
       <c r="S83" s="4" t="n">
         <f aca="false">SUM(M83:R83)</f>
-        <v>6875</v>
+        <v>6950</v>
       </c>
       <c r="T83" s="3"/>
       <c r="U83" s="24" t="n">
@@ -7015,11 +7026,11 @@
       </c>
       <c r="Z83" s="24" t="n">
         <f aca="false">SUM(Z4:Z82)</f>
-        <v>18</v>
+        <v>18.75</v>
       </c>
       <c r="AA83" s="24" t="n">
         <f aca="false">SUM(U83:Z83)</f>
-        <v>68.75</v>
+        <v>69.5</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Syncing from share - 4/17 and updating submodule
</commit_message>
<xml_diff>
--- a/team_folder/newFolder/Project Management/Logging/Burn Report.xlsx
+++ b/team_folder/newFolder/Project Management/Logging/Burn Report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
   <si>
     <t xml:space="preserve">Per Person</t>
   </si>
@@ -239,6 +239,27 @@
   </si>
   <si>
     <t xml:space="preserve">Begun initial work on web interface of rover with straight, left, right, backward, and 360 buttons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUI - Movement Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finished encoder test bench.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED Integration and function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Led VHDL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify C function, wrapper, and functional test logic</t>
   </si>
   <si>
     <t xml:space="preserve">Total CDR Costs</t>
@@ -797,25 +818,25 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B41" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
-      <selection pane="topRight" activeCell="I60" activeCellId="0" sqref="I60"/>
+      <selection pane="topRight" activeCell="I65" activeCellId="0" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="0" width="9.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="15" min="13" style="0" width="9.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="15" min="13" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="17" min="16" style="0" width="8.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="18" min="18" style="0" width="9.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="18" min="18" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="19" min="19" style="0" width="17.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="21" min="21" style="0" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="22" min="22" style="0" width="6"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="23" min="23" style="0" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="23" min="23" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="24" min="24" style="0" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="26" min="25" style="0" width="6"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="27" min="27" style="0" width="17.71"/>
@@ -1116,19 +1137,19 @@
       </c>
       <c r="AF4" s="19" t="n">
         <f aca="false">O83-AF3</f>
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="AG4" s="19" t="n">
         <f aca="false">P83-AG3</f>
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="AH4" s="19" t="n">
         <f aca="false">Q83-AH3</f>
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="AI4" s="19" t="n">
         <f aca="false">R83-AI3</f>
-        <v>1025</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1399,11 +1420,11 @@
       </c>
       <c r="AF7" s="29" t="n">
         <f aca="false">W83-AF6</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AG7" s="29" t="n">
         <f aca="false">X83-AG6</f>
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="AH7" s="29" t="n">
         <f aca="false">Y83-AH6</f>
@@ -1411,7 +1432,7 @@
       </c>
       <c r="AI7" s="29" t="n">
         <f aca="false">Z83-AI6</f>
-        <v>10.25</v>
+        <v>13.25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1578,19 +1599,19 @@
       </c>
       <c r="AF9" s="19" t="n">
         <f aca="false">SUM(AF3+AF4)</f>
-        <v>250</v>
+        <v>650</v>
       </c>
       <c r="AG9" s="19" t="n">
         <f aca="false">SUM(AG3+AG4)</f>
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="AH9" s="19" t="n">
         <f aca="false">SUM(AH3+AH4)</f>
-        <v>650</v>
+        <v>750</v>
       </c>
       <c r="AI9" s="19" t="n">
         <f aca="false">SUM(AI3+AI4)</f>
-        <v>1875</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1680,11 +1701,11 @@
       </c>
       <c r="AF10" s="29" t="n">
         <f aca="false">SUM(AF6+AF7)</f>
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="AG10" s="29" t="n">
         <f aca="false">SUM(AG6+AG7)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AH10" s="29" t="n">
         <f aca="false">SUM(AH6+AH7)</f>
@@ -1692,7 +1713,7 @@
       </c>
       <c r="AI10" s="29" t="n">
         <f aca="false">SUM(AI6+AI7)</f>
-        <v>18.75</v>
+        <v>21.75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4934,7 +4955,7 @@
       </c>
       <c r="AA53" s="3"/>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="25" t="n">
         <v>43201</v>
       </c>
@@ -5009,7 +5030,7 @@
       </c>
       <c r="AA54" s="3"/>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="25" t="n">
         <v>43204</v>
       </c>
@@ -5054,7 +5075,7 @@
       </c>
       <c r="R55" s="3" t="n">
         <f aca="false">IF(I55=1,100*$C55,0)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
@@ -5080,11 +5101,11 @@
       </c>
       <c r="Z55" s="24" t="n">
         <f aca="false">IF(I55=1,$C55,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA55" s="3"/>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="25" t="n">
         <v>43206</v>
       </c>
@@ -5159,7 +5180,7 @@
       </c>
       <c r="AA56" s="3"/>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="25" t="n">
         <v>43206</v>
       </c>
@@ -5234,7 +5255,7 @@
       </c>
       <c r="AA57" s="3"/>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="25" t="n">
         <v>43206</v>
       </c>
@@ -5309,7 +5330,7 @@
       </c>
       <c r="AA58" s="3"/>
     </row>
-    <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="25" t="n">
         <v>43207</v>
       </c>
@@ -5385,18 +5406,26 @@
       <c r="AA59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="25"/>
-      <c r="B60" s="28"/>
-      <c r="C60" s="23"/>
+      <c r="A60" s="25" t="n">
+        <v>43207</v>
+      </c>
+      <c r="B60" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C60" s="23" t="n">
+        <v>2</v>
+      </c>
       <c r="D60" s="33"/>
       <c r="E60" s="33"/>
       <c r="F60" s="33"/>
-      <c r="G60" s="33"/>
+      <c r="G60" s="33" t="n">
+        <v>1</v>
+      </c>
       <c r="H60" s="33"/>
       <c r="I60" s="33"/>
       <c r="J60" s="18" t="n">
         <f aca="false">SUM(D60:I60)*100*C60</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="L60" s="3"/>
       <c r="M60" s="3" t="n">
@@ -5413,7 +5442,7 @@
       </c>
       <c r="P60" s="3" t="n">
         <f aca="false">IF(G60=1,100*$C60,0)</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="Q60" s="3" t="n">
         <f aca="false">IF(H60=1,100*$C60,0)</f>
@@ -5439,7 +5468,7 @@
       </c>
       <c r="X60" s="24" t="n">
         <f aca="false">IF(G60=1,$C60,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y60" s="24" t="n">
         <f aca="false">IF(H60=1,$C60,0)</f>
@@ -5452,18 +5481,26 @@
       <c r="AA60" s="3"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="25"/>
-      <c r="B61" s="28"/>
-      <c r="C61" s="23"/>
+      <c r="A61" s="25" t="n">
+        <v>43207</v>
+      </c>
+      <c r="B61" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" s="23" t="s">
+        <v>75</v>
+      </c>
       <c r="D61" s="33"/>
       <c r="E61" s="33"/>
       <c r="F61" s="33"/>
       <c r="G61" s="33"/>
-      <c r="H61" s="33"/>
+      <c r="H61" s="33" t="n">
+        <v>1</v>
+      </c>
       <c r="I61" s="33"/>
       <c r="J61" s="18" t="n">
         <f aca="false">SUM(D61:I61)*100*C61</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L61" s="3"/>
       <c r="M61" s="3" t="n">
@@ -5484,7 +5521,7 @@
       </c>
       <c r="Q61" s="3" t="n">
         <f aca="false">IF(H61=1,100*$C61,0)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="R61" s="3" t="n">
         <f aca="false">IF(I61=1,100*$C61,0)</f>
@@ -5508,9 +5545,9 @@
         <f aca="false">IF(G61=1,$C61,0)</f>
         <v>0</v>
       </c>
-      <c r="Y61" s="24" t="n">
+      <c r="Y61" s="24" t="str">
         <f aca="false">IF(H61=1,$C61,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z61" s="24" t="n">
         <f aca="false">IF(I61=1,$C61,0)</f>
@@ -5519,18 +5556,26 @@
       <c r="AA61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="25"/>
-      <c r="B62" s="28"/>
-      <c r="C62" s="23"/>
+      <c r="A62" s="25" t="n">
+        <v>43207</v>
+      </c>
+      <c r="B62" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" s="23" t="n">
+        <v>2</v>
+      </c>
       <c r="D62" s="33"/>
       <c r="E62" s="33"/>
-      <c r="F62" s="33"/>
+      <c r="F62" s="33" t="n">
+        <v>1</v>
+      </c>
       <c r="G62" s="33"/>
       <c r="H62" s="33"/>
       <c r="I62" s="33"/>
       <c r="J62" s="18" t="n">
         <f aca="false">SUM(D62:I62)*100*C62</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="L62" s="3"/>
       <c r="M62" s="3" t="n">
@@ -5543,7 +5588,7 @@
       </c>
       <c r="O62" s="3" t="n">
         <f aca="false">IF(F62=1,100*$C62,0)</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="P62" s="3" t="n">
         <f aca="false">IF(G62=1,100*$C62,0)</f>
@@ -5569,7 +5614,7 @@
       </c>
       <c r="W62" s="24" t="n">
         <f aca="false">IF(F62=1,$C62,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X62" s="24" t="n">
         <f aca="false">IF(G62=1,$C62,0)</f>
@@ -5586,18 +5631,26 @@
       <c r="AA62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="25"/>
-      <c r="B63" s="28"/>
-      <c r="C63" s="23"/>
+      <c r="A63" s="25" t="n">
+        <v>43207</v>
+      </c>
+      <c r="B63" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C63" s="23" t="s">
+        <v>78</v>
+      </c>
       <c r="D63" s="33"/>
       <c r="E63" s="33"/>
-      <c r="F63" s="33"/>
+      <c r="F63" s="33" t="n">
+        <v>1</v>
+      </c>
       <c r="G63" s="33"/>
       <c r="H63" s="33"/>
       <c r="I63" s="33"/>
       <c r="J63" s="18" t="n">
         <f aca="false">SUM(D63:I63)*100*C63</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="L63" s="3"/>
       <c r="M63" s="3" t="n">
@@ -5610,7 +5663,7 @@
       </c>
       <c r="O63" s="3" t="n">
         <f aca="false">IF(F63=1,100*$C63,0)</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="P63" s="3" t="n">
         <f aca="false">IF(G63=1,100*$C63,0)</f>
@@ -5634,9 +5687,9 @@
         <f aca="false">IF(E63=1,$C63,0)</f>
         <v>0</v>
       </c>
-      <c r="W63" s="24" t="n">
+      <c r="W63" s="24" t="str">
         <f aca="false">IF(F63=1,$C63,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X63" s="24" t="n">
         <f aca="false">IF(G63=1,$C63,0)</f>
@@ -5652,19 +5705,27 @@
       </c>
       <c r="AA63" s="3"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="25"/>
-      <c r="B64" s="28"/>
-      <c r="C64" s="23"/>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="25" t="n">
+        <v>43207</v>
+      </c>
+      <c r="B64" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C64" s="23" t="n">
+        <v>2</v>
+      </c>
       <c r="D64" s="33"/>
       <c r="E64" s="33"/>
       <c r="F64" s="33"/>
       <c r="G64" s="33"/>
       <c r="H64" s="33"/>
-      <c r="I64" s="33"/>
+      <c r="I64" s="33" t="n">
+        <v>1</v>
+      </c>
       <c r="J64" s="18" t="n">
         <f aca="false">SUM(D64:I64)*100*C64</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="L64" s="3"/>
       <c r="M64" s="3" t="n">
@@ -5689,7 +5750,7 @@
       </c>
       <c r="R64" s="3" t="n">
         <f aca="false">IF(I64=1,100*$C64,0)</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="S64" s="3"/>
       <c r="T64" s="3"/>
@@ -5715,7 +5776,7 @@
       </c>
       <c r="Z64" s="24" t="n">
         <f aca="false">IF(I64=1,$C64,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA64" s="3"/>
     </row>
@@ -6563,7 +6624,7 @@
         <v>0</v>
       </c>
       <c r="S77" s="6" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="T77" s="3"/>
       <c r="U77" s="24" t="n">
@@ -6591,7 +6652,7 @@
         <v>0</v>
       </c>
       <c r="AA77" s="6" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6635,7 +6696,7 @@
       </c>
       <c r="S78" s="4" t="n">
         <f aca="false">S83-S43</f>
-        <v>1825</v>
+        <v>2825</v>
       </c>
       <c r="T78" s="3"/>
       <c r="U78" s="24" t="n">
@@ -6664,7 +6725,7 @@
       </c>
       <c r="AA78" s="3" t="n">
         <f aca="false">AA83-AA43</f>
-        <v>18.25</v>
+        <v>25.25</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6938,11 +6999,11 @@
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="35"/>
       <c r="B83" s="36" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C83" s="37" t="n">
         <f aca="false">SUM(C3:C82)</f>
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D83" s="38" t="n">
         <f aca="false">U$83</f>
@@ -6954,11 +7015,11 @@
       </c>
       <c r="F83" s="38" t="n">
         <f aca="false">W$83</f>
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="G83" s="38" t="n">
         <f aca="false">X$83</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H83" s="38" t="n">
         <f aca="false">Y$83</f>
@@ -6966,14 +7027,14 @@
       </c>
       <c r="I83" s="38" t="n">
         <f aca="false">Z$83</f>
-        <v>18.75</v>
+        <v>21.75</v>
       </c>
       <c r="J83" s="39" t="n">
         <f aca="false">SUM(J3:J82)</f>
-        <v>7050</v>
+        <v>7950</v>
       </c>
       <c r="L83" s="3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="M83" s="4" t="n">
         <f aca="false">SUM(M3:M82)</f>
@@ -6985,23 +7046,23 @@
       </c>
       <c r="O83" s="4" t="n">
         <f aca="false">SUM(O3:O82)</f>
-        <v>250</v>
+        <v>650</v>
       </c>
       <c r="P83" s="4" t="n">
         <f aca="false">SUM(P3:P82)</f>
-        <v>800</v>
+        <v>1000</v>
       </c>
       <c r="Q83" s="4" t="n">
         <f aca="false">SUM(Q3:Q82)</f>
-        <v>650</v>
+        <v>750</v>
       </c>
       <c r="R83" s="4" t="n">
         <f aca="false">SUM(R3:R82)</f>
-        <v>1875</v>
+        <v>2175</v>
       </c>
       <c r="S83" s="4" t="n">
         <f aca="false">SUM(M83:R83)</f>
-        <v>6950</v>
+        <v>7950</v>
       </c>
       <c r="T83" s="3"/>
       <c r="U83" s="24" t="n">
@@ -7014,11 +7075,11 @@
       </c>
       <c r="W83" s="24" t="n">
         <f aca="false">SUM(W4:W82)</f>
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="X83" s="24" t="n">
         <f aca="false">SUM(X4:X82)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Y83" s="24" t="n">
         <f aca="false">SUM(Y4:Y82)</f>
@@ -7026,11 +7087,11 @@
       </c>
       <c r="Z83" s="24" t="n">
         <f aca="false">SUM(Z4:Z82)</f>
-        <v>18.75</v>
+        <v>21.75</v>
       </c>
       <c r="AA83" s="24" t="n">
         <f aca="false">SUM(U83:Z83)</f>
-        <v>69.5</v>
+        <v>76.5</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Updated submodule functions and burn report
</commit_message>
<xml_diff>
--- a/team_folder/newFolder/Project Management/Logging/Burn Report.xlsx
+++ b/team_folder/newFolder/Project Management/Logging/Burn Report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="83">
   <si>
     <t xml:space="preserve">Per Person</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t xml:space="preserve">Verify C function, wrapper, and functional test logic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refactored C and python wrapper functions</t>
   </si>
   <si>
     <t xml:space="preserve">Total CDR Costs</t>
@@ -818,7 +821,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B41" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
-      <selection pane="topRight" activeCell="I65" activeCellId="0" sqref="I65"/>
+      <selection pane="topRight" activeCell="I66" activeCellId="0" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
@@ -826,17 +829,17 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="0" width="9.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="0" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="15" min="13" style="0" width="9.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="15" min="13" style="0" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="17" min="16" style="0" width="8.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="18" min="18" style="0" width="9.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="18" min="18" style="0" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="1" max="19" min="19" style="0" width="17.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="21" min="21" style="0" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="22" min="22" style="0" width="6"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="23" min="23" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="23" min="23" style="0" width="8.7"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="24" min="24" style="0" width="5.57"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="26" min="25" style="0" width="6"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="27" min="27" style="0" width="17.71"/>
@@ -1149,7 +1152,7 @@
       </c>
       <c r="AI4" s="19" t="n">
         <f aca="false">R83-AI3</f>
-        <v>1325</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1432,7 +1435,7 @@
       </c>
       <c r="AI7" s="29" t="n">
         <f aca="false">Z83-AI6</f>
-        <v>13.25</v>
+        <v>14.25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1611,7 +1614,7 @@
       </c>
       <c r="AI9" s="19" t="n">
         <f aca="false">SUM(AI3+AI4)</f>
-        <v>2175</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1713,7 +1716,7 @@
       </c>
       <c r="AI10" s="29" t="n">
         <f aca="false">SUM(AI6+AI7)</f>
-        <v>21.75</v>
+        <v>22.75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5780,19 +5783,27 @@
       </c>
       <c r="AA64" s="3"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="25"/>
-      <c r="B65" s="28"/>
-      <c r="C65" s="23"/>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="25" t="n">
+        <v>43208</v>
+      </c>
+      <c r="B65" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C65" s="23" t="n">
+        <v>1</v>
+      </c>
       <c r="D65" s="33"/>
       <c r="E65" s="33"/>
       <c r="F65" s="33"/>
       <c r="G65" s="33"/>
       <c r="H65" s="33"/>
-      <c r="I65" s="33"/>
+      <c r="I65" s="33" t="n">
+        <v>1</v>
+      </c>
       <c r="J65" s="18" t="n">
         <f aca="false">SUM(D65:I65)*100*C65</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L65" s="3"/>
       <c r="M65" s="3" t="n">
@@ -5817,7 +5828,7 @@
       </c>
       <c r="R65" s="3" t="n">
         <f aca="false">IF(I65=1,100*$C65,0)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S65" s="3"/>
       <c r="T65" s="3"/>
@@ -5843,7 +5854,7 @@
       </c>
       <c r="Z65" s="24" t="n">
         <f aca="false">IF(I65=1,$C65,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA65" s="3"/>
     </row>
@@ -6624,7 +6635,7 @@
         <v>0</v>
       </c>
       <c r="S77" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="T77" s="3"/>
       <c r="U77" s="24" t="n">
@@ -6652,7 +6663,7 @@
         <v>0</v>
       </c>
       <c r="AA77" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6696,7 +6707,7 @@
       </c>
       <c r="S78" s="4" t="n">
         <f aca="false">S83-S43</f>
-        <v>2825</v>
+        <v>2925</v>
       </c>
       <c r="T78" s="3"/>
       <c r="U78" s="24" t="n">
@@ -6725,7 +6736,7 @@
       </c>
       <c r="AA78" s="3" t="n">
         <f aca="false">AA83-AA43</f>
-        <v>25.25</v>
+        <v>26.25</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6999,11 +7010,11 @@
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="35"/>
       <c r="B83" s="36" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C83" s="37" t="n">
         <f aca="false">SUM(C3:C82)</f>
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D83" s="38" t="n">
         <f aca="false">U$83</f>
@@ -7027,14 +7038,14 @@
       </c>
       <c r="I83" s="38" t="n">
         <f aca="false">Z$83</f>
-        <v>21.75</v>
+        <v>22.75</v>
       </c>
       <c r="J83" s="39" t="n">
         <f aca="false">SUM(J3:J82)</f>
-        <v>7950</v>
+        <v>8050</v>
       </c>
       <c r="L83" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M83" s="4" t="n">
         <f aca="false">SUM(M3:M82)</f>
@@ -7058,11 +7069,11 @@
       </c>
       <c r="R83" s="4" t="n">
         <f aca="false">SUM(R3:R82)</f>
-        <v>2175</v>
+        <v>2275</v>
       </c>
       <c r="S83" s="4" t="n">
         <f aca="false">SUM(M83:R83)</f>
-        <v>7950</v>
+        <v>8050</v>
       </c>
       <c r="T83" s="3"/>
       <c r="U83" s="24" t="n">
@@ -7087,11 +7098,11 @@
       </c>
       <c r="Z83" s="24" t="n">
         <f aca="false">SUM(Z4:Z82)</f>
-        <v>21.75</v>
+        <v>22.75</v>
       </c>
       <c r="AA83" s="24" t="n">
         <f aca="false">SUM(U83:Z83)</f>
-        <v>76.5</v>
+        <v>77.5</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added diagrams and burn report
</commit_message>
<xml_diff>
--- a/team_folder/newFolder/Project Management/Logging/Burn Report.xlsx
+++ b/team_folder/newFolder/Project Management/Logging/Burn Report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="85">
   <si>
     <t xml:space="preserve">Per Person</t>
   </si>
@@ -263,6 +263,12 @@
   </si>
   <si>
     <t xml:space="preserve">Refactored C and python wrapper functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adjusted C offsets, tested wk 13 blink axi on rover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documented diagrams of functional tests and web interface</t>
   </si>
   <si>
     <t xml:space="preserve">Total CDR Costs</t>
@@ -821,7 +827,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B41" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
-      <selection pane="topRight" activeCell="I66" activeCellId="0" sqref="I66"/>
+      <selection pane="topRight" activeCell="I68" activeCellId="0" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
@@ -1152,7 +1158,7 @@
       </c>
       <c r="AI4" s="19" t="n">
         <f aca="false">R83-AI3</f>
-        <v>1425</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1435,7 +1441,7 @@
       </c>
       <c r="AI7" s="29" t="n">
         <f aca="false">Z83-AI6</f>
-        <v>14.25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1614,7 +1620,7 @@
       </c>
       <c r="AI9" s="19" t="n">
         <f aca="false">SUM(AI3+AI4)</f>
-        <v>2275</v>
+        <v>2450</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1716,7 +1722,7 @@
       </c>
       <c r="AI10" s="29" t="n">
         <f aca="false">SUM(AI6+AI7)</f>
-        <v>22.75</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5858,19 +5864,27 @@
       </c>
       <c r="AA65" s="3"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="25"/>
-      <c r="B66" s="28"/>
-      <c r="C66" s="23"/>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="25" t="n">
+        <v>43208</v>
+      </c>
+      <c r="B66" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C66" s="23" t="n">
+        <v>1.5</v>
+      </c>
       <c r="D66" s="33"/>
       <c r="E66" s="33"/>
       <c r="F66" s="33"/>
       <c r="G66" s="33"/>
       <c r="H66" s="33"/>
-      <c r="I66" s="33"/>
+      <c r="I66" s="33" t="n">
+        <v>1</v>
+      </c>
       <c r="J66" s="18" t="n">
         <f aca="false">SUM(D66:I66)*100*C66</f>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="L66" s="3"/>
       <c r="M66" s="3" t="n">
@@ -5895,7 +5909,7 @@
       </c>
       <c r="R66" s="3" t="n">
         <f aca="false">IF(I66=1,100*$C66,0)</f>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="S66" s="3"/>
       <c r="T66" s="3"/>
@@ -5921,23 +5935,31 @@
       </c>
       <c r="Z66" s="24" t="n">
         <f aca="false">IF(I66=1,$C66,0)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AA66" s="6"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="25"/>
-      <c r="B67" s="28"/>
-      <c r="C67" s="23"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="25" t="n">
+        <v>43208</v>
+      </c>
+      <c r="B67" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67" s="23" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D67" s="33"/>
       <c r="E67" s="33"/>
       <c r="F67" s="33"/>
       <c r="G67" s="33"/>
       <c r="H67" s="33"/>
-      <c r="I67" s="33"/>
+      <c r="I67" s="33" t="n">
+        <v>1</v>
+      </c>
       <c r="J67" s="18" t="n">
         <f aca="false">SUM(D67:I67)*100*C67</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="L67" s="3"/>
       <c r="M67" s="3" t="n">
@@ -5962,7 +5984,7 @@
       </c>
       <c r="R67" s="3" t="n">
         <f aca="false">IF(I67=1,100*$C67,0)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="S67" s="3"/>
       <c r="T67" s="3"/>
@@ -5988,7 +6010,7 @@
       </c>
       <c r="Z67" s="24" t="n">
         <f aca="false">IF(I67=1,$C67,0)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="AA67" s="4"/>
     </row>
@@ -6635,7 +6657,7 @@
         <v>0</v>
       </c>
       <c r="S77" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="T77" s="3"/>
       <c r="U77" s="24" t="n">
@@ -6663,7 +6685,7 @@
         <v>0</v>
       </c>
       <c r="AA77" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6707,7 +6729,7 @@
       </c>
       <c r="S78" s="4" t="n">
         <f aca="false">S83-S43</f>
-        <v>2925</v>
+        <v>3100</v>
       </c>
       <c r="T78" s="3"/>
       <c r="U78" s="24" t="n">
@@ -6736,7 +6758,7 @@
       </c>
       <c r="AA78" s="3" t="n">
         <f aca="false">AA83-AA43</f>
-        <v>26.25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7010,11 +7032,11 @@
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="35"/>
       <c r="B83" s="36" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C83" s="37" t="n">
         <f aca="false">SUM(C3:C82)</f>
-        <v>71</v>
+        <v>72.75</v>
       </c>
       <c r="D83" s="38" t="n">
         <f aca="false">U$83</f>
@@ -7038,14 +7060,14 @@
       </c>
       <c r="I83" s="38" t="n">
         <f aca="false">Z$83</f>
-        <v>22.75</v>
+        <v>24.5</v>
       </c>
       <c r="J83" s="39" t="n">
         <f aca="false">SUM(J3:J82)</f>
-        <v>8050</v>
+        <v>8225</v>
       </c>
       <c r="L83" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M83" s="4" t="n">
         <f aca="false">SUM(M3:M82)</f>
@@ -7069,11 +7091,11 @@
       </c>
       <c r="R83" s="4" t="n">
         <f aca="false">SUM(R3:R82)</f>
-        <v>2275</v>
+        <v>2450</v>
       </c>
       <c r="S83" s="4" t="n">
         <f aca="false">SUM(M83:R83)</f>
-        <v>8050</v>
+        <v>8225</v>
       </c>
       <c r="T83" s="3"/>
       <c r="U83" s="24" t="n">
@@ -7098,11 +7120,11 @@
       </c>
       <c r="Z83" s="24" t="n">
         <f aca="false">SUM(Z4:Z82)</f>
-        <v>22.75</v>
+        <v>24.5</v>
       </c>
       <c r="AA83" s="24" t="n">
         <f aca="false">SUM(U83:Z83)</f>
-        <v>77.5</v>
+        <v>79.25</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>